<commit_message>
Documentos revisados conforme a la revisión del profesor
</commit_message>
<xml_diff>
--- a/Plantilla Burndown.xlsx
+++ b/Plantilla Burndown.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alberto\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alberto\Desktop\Universidad\PGPI\Trabajo PGPI\Repositorio-PGPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2371,7 +2371,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="B2" sqref="B2:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Imágenes Burndown y documentos actualizados
</commit_message>
<xml_diff>
--- a/Plantilla Burndown.xlsx
+++ b/Plantilla Burndown.xlsx
@@ -24,12 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Día</t>
   </si>
   <si>
     <t>Puntos restantes</t>
+  </si>
+  <si>
+    <t>Contando 4 memorias, 4 veces que se sacan las graficas de burndown y 4 reuniones</t>
+  </si>
+  <si>
+    <t>a estos 10 puntos hay que restarle 2 por memoria, 2 por graficas y 1 por reunión con el cliente</t>
   </si>
 </sst>
 </file>
@@ -65,8 +71,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -123,7 +130,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 2)</a:t>
+              <a:t> 3)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -243,6 +250,9 @@
                 <c:pt idx="13">
                   <c:v>13</c:v>
                 </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -253,45 +263,48 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -319,7 +332,7 @@
         <c:axId val="1134209312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="13"/>
+          <c:max val="14"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -387,7 +400,7 @@
         <c:axId val="1234224016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="22"/>
+          <c:max val="70"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -446,7 +459,7 @@
         <c:crossAx val="1134209312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="2"/>
+        <c:majorUnit val="5"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -633,13 +646,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>126</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63</c:v>
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -734,7 +750,7 @@
         <c:axId val="1234224016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="126"/>
+          <c:max val="140"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -793,7 +809,7 @@
         <c:crossAx val="1134209312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="6"/>
+        <c:majorUnit val="10"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1987,9 +2003,9 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>291353</xdr:colOff>
+      <xdr:colOff>307398</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>78441</xdr:rowOff>
+      <xdr:rowOff>177511</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -2004,8 +2020,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3339353" y="649941"/>
-          <a:ext cx="4074272" cy="2191684"/>
+          <a:off x="3355398" y="749011"/>
+          <a:ext cx="4058227" cy="2092614"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2327,10 +2343,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2338,7 +2354,7 @@
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2352,26 +2368,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>22</v>
+        <v>67</v>
+      </c>
+      <c r="K2">
+        <f>126-85</f>
+        <v>41</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>126</v>
+        <v>140</v>
+      </c>
+      <c r="O2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="K3">
         <f>1+1+1+2+1+4+2+5+4+2+6+2+6+8+2+2+3+2</f>
@@ -2382,15 +2405,15 @@
       </c>
       <c r="N3">
         <f>N2-41</f>
-        <v>85</v>
+        <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="K4">
         <f>K3-2-3-8</f>
@@ -2401,15 +2424,15 @@
       </c>
       <c r="N4">
         <f>N3-22</f>
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="K5">
         <f>1+1+1+2+1+4+2+5+4+2+6+2+6+2+2</f>
@@ -2418,94 +2441,124 @@
       <c r="M5">
         <v>3</v>
       </c>
+      <c r="N5">
+        <f>N4-67</f>
+        <v>10</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="M6">
         <v>4</v>
       </c>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="M7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f>2+8+5+8+5+8+5+8+5+8+5</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27">
         <f>1+1+1+2+1+4+2+4+4+2+5+4+2+1+2+6+2+2+8+5+8+5+8+5+8+5+8+5+10+3+2</f>
         <v>126</v>

</xml_diff>